<commit_message>
large update all files
</commit_message>
<xml_diff>
--- a/Fig.4/Fig.4.LiP.DODO.xlsx
+++ b/Fig.4/Fig.4.LiP.DODO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://merced-my.sharepoint.com/personal/ssukenik_ucmerced_edu/Documents/Collabs/Fried/Github/Romero_Surface_Desiccation/Fig.4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stephenfried/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B3EA0CDB-A620-44D6-A300-532718CA3F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B28E06F5-46B8-4A4F-BB16-03E41DAAC2D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12432" xr2:uid="{C750A44D-7B1C-AB4D-B751-E79D7DECC915}"/>
+    <workbookView xWindow="3400" yWindow="2360" windowWidth="26840" windowHeight="15940" activeTab="5" xr2:uid="{C750A44D-7B1C-AB4D-B751-E79D7DECC915}"/>
   </bookViews>
   <sheets>
     <sheet name="percentDE" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
   <si>
     <t>proteins structurall retained</t>
   </si>
@@ -79,9 +79,15 @@
     <t>30-35%</t>
   </si>
   <si>
+    <t>35%+</t>
+  </si>
+  <si>
     <t>35-40%</t>
   </si>
   <si>
+    <t>40%+</t>
+  </si>
+  <si>
     <t>0-1%</t>
   </si>
   <si>
@@ -97,16 +103,10 @@
     <t>6-8%</t>
   </si>
   <si>
-    <t>&gt; 8%</t>
-  </si>
-  <si>
-    <t>&gt;35%</t>
-  </si>
-  <si>
-    <t>&gt;40%</t>
-  </si>
-  <si>
-    <t>&gt;30%</t>
+    <t>8-10%</t>
+  </si>
+  <si>
+    <t>10%+</t>
   </si>
 </sst>
 </file>
@@ -154,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -211,11 +211,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -226,6 +257,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,15 +595,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357CB0CD-500C-BB43-8935-1136215186DB}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -585,124 +620,158 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>13</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>10</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D3" s="7">
         <v>46</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E3" s="9">
         <v>316</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>0.14556962025316456</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="4">
         <v>56</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C4" s="5">
         <v>31</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4" s="7">
         <v>157</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E4" s="9">
         <v>1160</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>0.13534482758620689</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="4">
         <v>252</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <v>94</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D5" s="7">
         <v>505</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E5" s="9">
         <v>5511</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>9.1634911994193435E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>330</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="5">
         <v>83</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6" s="7">
         <v>502</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E6" s="9">
         <v>7494</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>6.6986922871630633E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="4">
         <v>133</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>27</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7" s="7">
         <v>157</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E7" s="9">
         <v>3453</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>4.5467709238343472E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4">
-        <v>27</v>
-      </c>
-      <c r="C7" s="5">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7">
-        <v>20</v>
-      </c>
-      <c r="E7" s="9">
-        <v>289</v>
-      </c>
-      <c r="F7">
-        <v>6.9204152249134954E-2</v>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4">
+        <v>22</v>
+      </c>
+      <c r="C8" s="5">
+        <v>3</v>
+      </c>
+      <c r="D8" s="7">
+        <v>13</v>
+      </c>
+      <c r="E8" s="9">
+        <v>250</v>
+      </c>
+      <c r="F8">
+        <v>5.1999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="7">
+        <v>7</v>
+      </c>
+      <c r="E9" s="9">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -712,15 +781,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D48FFE2-8F03-604A-BFB9-F59A528CA946}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -737,124 +806,158 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B3" s="4">
         <v>30</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C3" s="5">
         <v>4</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D3" s="7">
         <v>18</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E3" s="9">
         <v>294</v>
       </c>
-      <c r="F2">
+      <c r="F3">
         <v>6.1224489795918366E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B4" s="4">
         <v>186</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C4" s="5">
         <v>47</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D4" s="7">
         <v>294</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E4" s="9">
         <v>3736</v>
       </c>
-      <c r="F3">
+      <c r="F4">
         <v>7.8693790149892931E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B5" s="4">
         <v>404</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C5" s="5">
         <v>124</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D5" s="7">
         <v>663</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E5" s="9">
         <v>10146</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>6.5345949142519219E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A5" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <v>157</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C6" s="5">
         <v>55</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D6" s="7">
         <v>341</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E6" s="9">
         <v>3483</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>9.7904105656043641E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B7" s="4">
         <v>30</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C7" s="5">
         <v>13</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D7" s="7">
         <v>38</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E7" s="9">
         <v>371</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>0.10242587601078167</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A7" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="5">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7">
         <v>21</v>
       </c>
-      <c r="B7" s="4">
-        <v>4</v>
-      </c>
-      <c r="C7" s="5">
-        <v>6</v>
-      </c>
-      <c r="D7" s="7">
-        <v>32</v>
-      </c>
-      <c r="E7" s="9">
-        <v>194</v>
-      </c>
-      <c r="F7">
-        <v>0.16494845360824742</v>
+      <c r="E8" s="9">
+        <v>173</v>
+      </c>
+      <c r="F8">
+        <v>0.12138728323699421</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>2</v>
+      </c>
+      <c r="D9" s="7">
+        <v>11</v>
+      </c>
+      <c r="E9" s="9">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -864,15 +967,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{898D39EB-7BD8-6E49-93B3-605E506A6B1F}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -889,7 +992,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -906,7 +1009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -926,7 +1029,7 @@
         <v>0.14814814814814814</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -946,7 +1049,7 @@
         <v>0.18289085545722714</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -966,7 +1069,7 @@
         <v>0.15796640944167045</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -986,7 +1089,7 @@
         <v>6.895273401297497E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -1006,7 +1109,7 @@
         <v>6.3416422287390029E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
@@ -1026,24 +1129,41 @@
         <v>3.5835214446952597E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B9" s="4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D9" s="7">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E9" s="9">
-        <v>868</v>
+        <v>790</v>
       </c>
       <c r="F9">
-        <v>6.6820276497695855E-2</v>
+        <v>5.8227848101265821E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
+        <v>2</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="7">
+        <v>12</v>
+      </c>
+      <c r="E10" s="9">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1053,15 +1173,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{679B437B-A655-AA49-983A-6913B5C49B1B}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD9"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1078,9 +1198,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" s="2">
         <v>37</v>
@@ -1098,9 +1218,9 @@
         <v>4.6477850399419027E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>133</v>
@@ -1118,9 +1238,9 @@
         <v>7.7063661285409688E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4">
         <v>331</v>
@@ -1138,9 +1258,9 @@
         <v>6.4508697154705683E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="4">
         <v>197</v>
@@ -1158,9 +1278,9 @@
         <v>0.1080238162744542</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B6" s="4">
         <v>69</v>
@@ -1178,24 +1298,44 @@
         <v>7.8651685393258425E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C7" s="5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" s="7">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="E7" s="9">
-        <v>289</v>
+        <v>221</v>
       </c>
       <c r="F7">
-        <v>0.15570934256055363</v>
+        <v>0.13574660633484162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="10">
+        <v>6</v>
+      </c>
+      <c r="C8" s="11">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12">
+        <v>15</v>
+      </c>
+      <c r="E8" s="13">
+        <v>68</v>
+      </c>
+      <c r="F8">
+        <v>0.22058823529411764</v>
       </c>
     </row>
   </sheetData>
@@ -1205,15 +1345,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28E29197-4B10-DB49-80BE-054382B7928D}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1230,7 +1370,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1250,7 +1390,7 @@
         <v>5.8885383806519455E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1270,7 +1410,7 @@
         <v>6.2287148234450619E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -1290,7 +1430,7 @@
         <v>0.11351052048726468</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1308,6 +1448,94 @@
       </c>
       <c r="F5">
         <v>0.20370370370370369</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>8</v>
+      </c>
+      <c r="C6" s="5">
+        <v>1</v>
+      </c>
+      <c r="D6" s="7">
+        <v>3</v>
+      </c>
+      <c r="E6" s="9">
+        <v>55</v>
+      </c>
+      <c r="F6">
+        <v>5.4545454545454543E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>0</v>
+      </c>
+      <c r="C9" s="5">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0</v>
+      </c>
+      <c r="C10" s="5">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1317,15 +1545,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC1F376-FA73-FF48-8B6F-7F5587EA0375}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.6"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1342,143 +1570,177 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3">
+        <v>0</v>
+      </c>
+      <c r="D2" s="6">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="4">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B4" s="4">
         <v>9</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C4" s="5">
         <v>7</v>
       </c>
-      <c r="D2" s="7">
+      <c r="D4" s="7">
         <v>34</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E4" s="9">
         <v>241</v>
       </c>
-      <c r="F2">
+      <c r="F4">
         <v>0.14107883817427386</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A3" s="1" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B5" s="4">
         <v>88</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C5" s="5">
         <v>26</v>
       </c>
-      <c r="D3" s="7">
+      <c r="D5" s="7">
         <v>167</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E5" s="9">
         <v>3362</v>
       </c>
-      <c r="F3">
+      <c r="F5">
         <v>4.9672813801308745E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A4" s="1" t="s">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B6" s="4">
         <v>245</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C6" s="5">
         <v>81</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D6" s="7">
         <v>446</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E6" s="9">
         <v>6946</v>
       </c>
-      <c r="F4">
+      <c r="F6">
         <v>6.420961704578175E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A5" s="1" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B7" s="4">
         <v>269</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C7" s="5">
         <v>87</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D7" s="7">
         <v>459</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E7" s="9">
         <v>5343</v>
       </c>
-      <c r="F5">
+      <c r="F7">
         <v>8.5906793935991016E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A6" s="1" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B8" s="4">
         <v>138</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C8" s="5">
         <v>38</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D8" s="7">
         <v>199</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E8" s="9">
         <v>1923</v>
       </c>
-      <c r="F6">
+      <c r="F8">
         <v>0.10348413936557463</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A7" s="1" t="s">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="4">
+        <v>50</v>
+      </c>
+      <c r="C9" s="5">
+        <v>7</v>
+      </c>
+      <c r="D9" s="7">
+        <v>42</v>
+      </c>
+      <c r="E9" s="9">
+        <v>297</v>
+      </c>
+      <c r="F9">
+        <v>0.14141414141414141</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="4">
         <v>12</v>
       </c>
-      <c r="B7" s="4">
-        <v>50</v>
-      </c>
-      <c r="C7" s="5">
-        <v>7</v>
-      </c>
-      <c r="D7" s="7">
-        <v>42</v>
-      </c>
-      <c r="E7" s="9">
-        <v>297</v>
-      </c>
-      <c r="F7">
-        <v>0.14141414141414141</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.6">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="4">
-        <v>12</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="C10" s="5">
         <v>3</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D10" s="7">
         <v>40</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E10" s="9">
         <v>113</v>
       </c>
-      <c r="F8">
+      <c r="F10">
         <v>0.35398230088495575</v>
       </c>
     </row>

</xml_diff>